<commit_message>
transaction service is added
</commit_message>
<xml_diff>
--- a/MicroService App/TCER Sheet.xlsx
+++ b/MicroService App/TCER Sheet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nagal\git\XYZRetailRepo\MicroService App\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF3C3C22-3370-4AB8-BFC7-05A92DF30A9B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F63A527-1848-4FD5-83DC-E961F322F32E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5388" yWindow="708" windowWidth="17280" windowHeight="8880" xr2:uid="{6144ADCF-C8D8-4E84-B20B-C8733E953893}"/>
+    <workbookView xWindow="5760" yWindow="1404" windowWidth="17280" windowHeight="8880" activeTab="2" xr2:uid="{6144ADCF-C8D8-4E84-B20B-C8733E953893}"/>
   </bookViews>
   <sheets>
     <sheet name="Customer Service" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="66">
   <si>
     <t>TCER</t>
   </si>
@@ -181,6 +181,60 @@
   </si>
   <si>
     <t>int number of rows affected</t>
+  </si>
+  <si>
+    <t>Transaction Service</t>
+  </si>
+  <si>
+    <t>saveTransaction(Transaction transaction)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Add transaction </t>
+  </si>
+  <si>
+    <t>saveTransactionByUserName(String name)</t>
+  </si>
+  <si>
+    <t>if any name is passed</t>
+  </si>
+  <si>
+    <t>saveTransactionByUserName(null)</t>
+  </si>
+  <si>
+    <t>null object is passed</t>
+  </si>
+  <si>
+    <t>getMaxTransactionId()</t>
+  </si>
+  <si>
+    <t>maximum no.of transactions done by customer</t>
+  </si>
+  <si>
+    <t>getAllTransaction()</t>
+  </si>
+  <si>
+    <t>List&lt;Transactions&gt;</t>
+  </si>
+  <si>
+    <t>if atleast one transaction exists</t>
+  </si>
+  <si>
+    <t>if no transaction is done</t>
+  </si>
+  <si>
+    <t>R005</t>
+  </si>
+  <si>
+    <t>getAllTransactionByName(String name)</t>
+  </si>
+  <si>
+    <t>getAllTransaction(String name)</t>
+  </si>
+  <si>
+    <t>if atleast one transaction exists for customer</t>
+  </si>
+  <si>
+    <t>if no transaction is done for customer</t>
   </si>
 </sst>
 </file>
@@ -600,7 +654,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D4355650-76DC-4C96-82FF-19574E7C057C}">
   <dimension ref="A1:G23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+    <sheetView topLeftCell="A5" workbookViewId="0">
       <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
@@ -1088,13 +1142,21 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5C584728-4E5E-41F2-AD66-7AE5DFCD2E40}">
-  <dimension ref="A1:F3"/>
+  <dimension ref="A1:F16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:F3"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="14.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="35.21875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="40.109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="38.109375" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="21" x14ac:dyDescent="0.4">
       <c r="A1" s="7" t="s">
@@ -1108,7 +1170,7 @@
     </row>
     <row r="2" spans="1:6" ht="18" x14ac:dyDescent="0.35">
       <c r="A2" s="8" t="s">
-        <v>6</v>
+        <v>48</v>
       </c>
       <c r="B2" s="8"/>
       <c r="C2" s="8"/>
@@ -1134,6 +1196,139 @@
       </c>
       <c r="F3" s="1" t="s">
         <v>14</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" t="s">
+        <v>49</v>
+      </c>
+      <c r="D4" t="b">
+        <v>1</v>
+      </c>
+      <c r="F4" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>13</v>
+      </c>
+      <c r="B7" t="s">
+        <v>8</v>
+      </c>
+      <c r="C7" t="s">
+        <v>51</v>
+      </c>
+      <c r="D7" t="b">
+        <v>1</v>
+      </c>
+      <c r="F7" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>13</v>
+      </c>
+      <c r="B8" t="s">
+        <v>11</v>
+      </c>
+      <c r="C8" t="s">
+        <v>53</v>
+      </c>
+      <c r="D8" t="b">
+        <v>0</v>
+      </c>
+      <c r="F8" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>22</v>
+      </c>
+      <c r="B10" t="s">
+        <v>8</v>
+      </c>
+      <c r="C10" t="s">
+        <v>55</v>
+      </c>
+      <c r="D10" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>27</v>
+      </c>
+      <c r="B12" t="s">
+        <v>8</v>
+      </c>
+      <c r="C12" t="s">
+        <v>57</v>
+      </c>
+      <c r="D12" t="s">
+        <v>58</v>
+      </c>
+      <c r="F12" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>27</v>
+      </c>
+      <c r="B13" t="s">
+        <v>11</v>
+      </c>
+      <c r="C13" t="s">
+        <v>57</v>
+      </c>
+      <c r="D13" t="s">
+        <v>12</v>
+      </c>
+      <c r="F13" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>61</v>
+      </c>
+      <c r="B15" t="s">
+        <v>8</v>
+      </c>
+      <c r="C15" t="s">
+        <v>62</v>
+      </c>
+      <c r="D15" t="s">
+        <v>58</v>
+      </c>
+      <c r="F15" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>61</v>
+      </c>
+      <c r="B16" t="s">
+        <v>11</v>
+      </c>
+      <c r="C16" t="s">
+        <v>63</v>
+      </c>
+      <c r="D16" t="s">
+        <v>12</v>
+      </c>
+      <c r="F16" t="s">
+        <v>65</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
transaction service dao tcer done
</commit_message>
<xml_diff>
--- a/MicroService App/TCER Sheet.xlsx
+++ b/MicroService App/TCER Sheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nagal\git\XYZRetailRepo\MicroService App\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F63A527-1848-4FD5-83DC-E961F322F32E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AACB9D86-1154-449F-9D65-76A03C4BF4CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="5760" yWindow="1404" windowWidth="17280" windowHeight="8880" activeTab="2" xr2:uid="{6144ADCF-C8D8-4E84-B20B-C8733E953893}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="188" uniqueCount="79">
   <si>
     <t>TCER</t>
   </si>
@@ -189,9 +189,6 @@
     <t>saveTransaction(Transaction transaction)</t>
   </si>
   <si>
-    <t xml:space="preserve">Add transaction </t>
-  </si>
-  <si>
     <t>saveTransactionByUserName(String name)</t>
   </si>
   <si>
@@ -207,9 +204,6 @@
     <t>getMaxTransactionId()</t>
   </si>
   <si>
-    <t>maximum no.of transactions done by customer</t>
-  </si>
-  <si>
     <t>getAllTransaction()</t>
   </si>
   <si>
@@ -235,13 +229,58 @@
   </si>
   <si>
     <t>if no transaction is done for customer</t>
+  </si>
+  <si>
+    <t>Transaction Dao</t>
+  </si>
+  <si>
+    <t>saveTransactionByUserName(String userName)</t>
+  </si>
+  <si>
+    <t>If transaction is saved</t>
+  </si>
+  <si>
+    <t>if transaction is not saved</t>
+  </si>
+  <si>
+    <t xml:space="preserve">if it  transaction is added </t>
+  </si>
+  <si>
+    <t xml:space="preserve">if it  transaction is not added </t>
+  </si>
+  <si>
+    <t>latest transaction id</t>
+  </si>
+  <si>
+    <t>getMaxTransaction()</t>
+  </si>
+  <si>
+    <t>latest Transaction id</t>
+  </si>
+  <si>
+    <t>to get recent transaction id</t>
+  </si>
+  <si>
+    <t>findAll()</t>
+  </si>
+  <si>
+    <t>List All transactions</t>
+  </si>
+  <si>
+    <t>if there is atleast one transaction done by using application</t>
+  </si>
+  <si>
+    <t>if there is transaction done by using application</t>
+  </si>
+  <si>
+    <t>List transactions of particular user</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -269,6 +308,12 @@
       <b/>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -1142,20 +1187,19 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5C584728-4E5E-41F2-AD66-7AE5DFCD2E40}">
-  <dimension ref="A1:F16"/>
+  <dimension ref="A1:F30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="D31" sqref="D31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="14.88671875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="11" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="35.21875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="40.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="40.109375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="13.33203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="38.109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="49.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="21" x14ac:dyDescent="0.4">
@@ -1212,7 +1256,24 @@
         <v>1</v>
       </c>
       <c r="F4" t="s">
-        <v>50</v>
+        <v>68</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C5" t="s">
+        <v>49</v>
+      </c>
+      <c r="D5" t="b">
+        <v>0</v>
+      </c>
+      <c r="F5" t="s">
+        <v>69</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
@@ -1223,13 +1284,13 @@
         <v>8</v>
       </c>
       <c r="C7" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D7" t="b">
         <v>1</v>
       </c>
       <c r="F7" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
@@ -1240,13 +1301,13 @@
         <v>11</v>
       </c>
       <c r="C8" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D8" t="b">
         <v>0</v>
       </c>
       <c r="F8" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
@@ -1257,10 +1318,13 @@
         <v>8</v>
       </c>
       <c r="C10" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D10" t="s">
-        <v>56</v>
+        <v>70</v>
+      </c>
+      <c r="F10" t="s">
+        <v>73</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.3">
@@ -1271,13 +1335,13 @@
         <v>8</v>
       </c>
       <c r="C12" t="s">
+        <v>55</v>
+      </c>
+      <c r="D12" t="s">
+        <v>56</v>
+      </c>
+      <c r="F12" t="s">
         <v>57</v>
-      </c>
-      <c r="D12" t="s">
-        <v>58</v>
-      </c>
-      <c r="F12" t="s">
-        <v>59</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.3">
@@ -1288,54 +1352,205 @@
         <v>11</v>
       </c>
       <c r="C13" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="D13" t="s">
         <v>12</v>
       </c>
       <c r="F13" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B15" t="s">
         <v>8</v>
       </c>
       <c r="C15" t="s">
+        <v>60</v>
+      </c>
+      <c r="D15" t="s">
+        <v>56</v>
+      </c>
+      <c r="F15" t="s">
         <v>62</v>
-      </c>
-      <c r="D15" t="s">
-        <v>58</v>
-      </c>
-      <c r="F15" t="s">
-        <v>64</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B16" t="s">
         <v>11</v>
       </c>
       <c r="C16" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="D16" t="s">
         <v>12</v>
       </c>
       <c r="F16" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" ht="18" x14ac:dyDescent="0.35">
+      <c r="A19" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="B19" s="8"/>
+      <c r="C19" s="8"/>
+      <c r="D19" s="8"/>
+      <c r="E19" s="8"/>
+      <c r="F19" s="8"/>
+    </row>
+    <row r="20" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A20" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F20" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>7</v>
+      </c>
+      <c r="B21" t="s">
+        <v>8</v>
+      </c>
+      <c r="C21" t="s">
         <v>65</v>
       </c>
+      <c r="D21" t="b">
+        <v>1</v>
+      </c>
+      <c r="F21" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>7</v>
+      </c>
+      <c r="B22" t="s">
+        <v>11</v>
+      </c>
+      <c r="C22" t="s">
+        <v>65</v>
+      </c>
+      <c r="D22" t="b">
+        <v>0</v>
+      </c>
+      <c r="F22" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
+        <v>13</v>
+      </c>
+      <c r="B24" t="s">
+        <v>8</v>
+      </c>
+      <c r="C24" t="s">
+        <v>71</v>
+      </c>
+      <c r="D24" t="s">
+        <v>72</v>
+      </c>
+      <c r="F24" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
+        <v>22</v>
+      </c>
+      <c r="B26" t="s">
+        <v>8</v>
+      </c>
+      <c r="C26" t="s">
+        <v>74</v>
+      </c>
+      <c r="D26" t="s">
+        <v>75</v>
+      </c>
+      <c r="F26" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
+        <v>22</v>
+      </c>
+      <c r="B27" t="s">
+        <v>11</v>
+      </c>
+      <c r="C27" t="s">
+        <v>74</v>
+      </c>
+      <c r="D27" t="s">
+        <v>12</v>
+      </c>
+      <c r="F27" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A29" t="s">
+        <v>27</v>
+      </c>
+      <c r="B29" t="s">
+        <v>8</v>
+      </c>
+      <c r="C29" t="s">
+        <v>65</v>
+      </c>
+      <c r="D29" t="s">
+        <v>78</v>
+      </c>
+      <c r="F29" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A30" t="s">
+        <v>27</v>
+      </c>
+      <c r="B30" t="s">
+        <v>11</v>
+      </c>
+      <c r="C30" t="s">
+        <v>65</v>
+      </c>
+      <c r="D30" t="s">
+        <v>12</v>
+      </c>
+      <c r="F30" t="s">
+        <v>63</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="3">
     <mergeCell ref="A1:F1"/>
     <mergeCell ref="A2:F2"/>
+    <mergeCell ref="A19:F19"/>
   </mergeCells>
+  <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
ItemDetail TCER is updated
</commit_message>
<xml_diff>
--- a/MicroService App/TCER Sheet.xlsx
+++ b/MicroService App/TCER Sheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nagal\git\XYZRetailRepo\MicroService App\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5546B942-C7C8-4B27-BED4-1A4BF79F64F1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59456DBE-CE6C-4461-A8E8-CDA1A34B432A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="5760" yWindow="1404" windowWidth="17280" windowHeight="8880" firstSheet="1" activeTab="3" xr2:uid="{6144ADCF-C8D8-4E84-B20B-C8733E953893}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="204" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="289" uniqueCount="109">
   <si>
     <t>TCER</t>
   </si>
@@ -280,6 +280,90 @@
   </si>
   <si>
     <t>ItemsCart Service</t>
+  </si>
+  <si>
+    <t>getAllItemDetails()</t>
+  </si>
+  <si>
+    <t xml:space="preserve">List&lt;ItemDetails&gt; </t>
+  </si>
+  <si>
+    <t>collects all the items available in store</t>
+  </si>
+  <si>
+    <t>if there is no item present at store</t>
+  </si>
+  <si>
+    <t>findByItemId(String itemId)</t>
+  </si>
+  <si>
+    <t>ItemDetails item</t>
+  </si>
+  <si>
+    <t>Returns the ItemDetail object with the provided id</t>
+  </si>
+  <si>
+    <t>If item id deos not exist in store</t>
+  </si>
+  <si>
+    <t>findByItemId_AndAvailableQuantity(String Item Id , int availabkeQuantity)</t>
+  </si>
+  <si>
+    <t>ItemDetail item</t>
+  </si>
+  <si>
+    <t>returns Item detail if the provided item id consists of required quantity</t>
+  </si>
+  <si>
+    <t>if item with required quantity is not available</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R004 </t>
+  </si>
+  <si>
+    <t>updateRecord(String itemId,int quantity)</t>
+  </si>
+  <si>
+    <t>updated ItemDetail</t>
+  </si>
+  <si>
+    <t>returns the updated item id by reducing the mentioned quantity</t>
+  </si>
+  <si>
+    <t>if it cannot update the quantity mentioned</t>
+  </si>
+  <si>
+    <t>ItemDetail Dao</t>
+  </si>
+  <si>
+    <t>List&lt;ItemDetail&gt;</t>
+  </si>
+  <si>
+    <t>returns the list of available items</t>
+  </si>
+  <si>
+    <t>empty list</t>
+  </si>
+  <si>
+    <t>if there exist no element</t>
+  </si>
+  <si>
+    <t>findById(String itemId)</t>
+  </si>
+  <si>
+    <t>ItemDetail</t>
+  </si>
+  <si>
+    <t>if item with item id exists</t>
+  </si>
+  <si>
+    <t>if item with item id does not exists</t>
+  </si>
+  <si>
+    <t>findByItemIdAndAvailableQuantity(String item id,int quantity)</t>
+  </si>
+  <si>
+    <t>if item id updated by reducing the mentioned quantity</t>
   </si>
 </sst>
 </file>
@@ -1563,20 +1647,20 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{77C7A937-846C-4C77-8D91-13859D3BE2A9}">
-  <dimension ref="A1:F3"/>
+  <dimension ref="A1:F28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="F30" sqref="F30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="14.88671875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="11" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.21875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="61.6640625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="15.88671875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="13.33203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="59" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="21" x14ac:dyDescent="0.4">
@@ -1619,11 +1703,315 @@
         <v>14</v>
       </c>
     </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" t="s">
+        <v>81</v>
+      </c>
+      <c r="D4" t="s">
+        <v>82</v>
+      </c>
+      <c r="F4" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C5" t="s">
+        <v>81</v>
+      </c>
+      <c r="D5" t="s">
+        <v>12</v>
+      </c>
+      <c r="F5" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>13</v>
+      </c>
+      <c r="B7" t="s">
+        <v>8</v>
+      </c>
+      <c r="C7" t="s">
+        <v>85</v>
+      </c>
+      <c r="D7" t="s">
+        <v>86</v>
+      </c>
+      <c r="F7" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>13</v>
+      </c>
+      <c r="B8" t="s">
+        <v>11</v>
+      </c>
+      <c r="C8" t="s">
+        <v>85</v>
+      </c>
+      <c r="D8" t="s">
+        <v>12</v>
+      </c>
+      <c r="F8" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>22</v>
+      </c>
+      <c r="B10" t="s">
+        <v>8</v>
+      </c>
+      <c r="C10" t="s">
+        <v>89</v>
+      </c>
+      <c r="D10" t="s">
+        <v>90</v>
+      </c>
+      <c r="F10" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>22</v>
+      </c>
+      <c r="B11" t="s">
+        <v>11</v>
+      </c>
+      <c r="C11" t="s">
+        <v>89</v>
+      </c>
+      <c r="D11" t="s">
+        <v>12</v>
+      </c>
+      <c r="F11" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>93</v>
+      </c>
+      <c r="B13" t="s">
+        <v>8</v>
+      </c>
+      <c r="C13" t="s">
+        <v>94</v>
+      </c>
+      <c r="D13" t="s">
+        <v>95</v>
+      </c>
+      <c r="F13" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>93</v>
+      </c>
+      <c r="B14" t="s">
+        <v>11</v>
+      </c>
+      <c r="C14" t="s">
+        <v>94</v>
+      </c>
+      <c r="D14" t="s">
+        <v>12</v>
+      </c>
+      <c r="F14" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" ht="18" x14ac:dyDescent="0.35">
+      <c r="A16" s="8" t="s">
+        <v>98</v>
+      </c>
+      <c r="B16" s="8"/>
+      <c r="C16" s="8"/>
+      <c r="D16" s="8"/>
+      <c r="E16" s="8"/>
+      <c r="F16" s="8"/>
+    </row>
+    <row r="17" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A17" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F17" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>7</v>
+      </c>
+      <c r="B18" t="s">
+        <v>8</v>
+      </c>
+      <c r="C18" t="s">
+        <v>74</v>
+      </c>
+      <c r="D18" t="s">
+        <v>99</v>
+      </c>
+      <c r="F18" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>7</v>
+      </c>
+      <c r="B19" t="s">
+        <v>11</v>
+      </c>
+      <c r="C19" t="s">
+        <v>74</v>
+      </c>
+      <c r="D19" t="s">
+        <v>101</v>
+      </c>
+      <c r="F19" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>13</v>
+      </c>
+      <c r="B21" t="s">
+        <v>8</v>
+      </c>
+      <c r="C21" t="s">
+        <v>103</v>
+      </c>
+      <c r="D21" t="s">
+        <v>104</v>
+      </c>
+      <c r="F21" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>13</v>
+      </c>
+      <c r="B22" t="s">
+        <v>11</v>
+      </c>
+      <c r="C22" t="s">
+        <v>103</v>
+      </c>
+      <c r="D22" t="s">
+        <v>12</v>
+      </c>
+      <c r="F22" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
+        <v>22</v>
+      </c>
+      <c r="B24" t="s">
+        <v>8</v>
+      </c>
+      <c r="C24" t="s">
+        <v>107</v>
+      </c>
+      <c r="D24" t="s">
+        <v>104</v>
+      </c>
+      <c r="F24" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
+        <v>22</v>
+      </c>
+      <c r="B25" t="s">
+        <v>11</v>
+      </c>
+      <c r="C25" t="s">
+        <v>107</v>
+      </c>
+      <c r="D25" t="s">
+        <v>12</v>
+      </c>
+      <c r="F25" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
+        <v>93</v>
+      </c>
+      <c r="B27" t="s">
+        <v>8</v>
+      </c>
+      <c r="C27" t="s">
+        <v>94</v>
+      </c>
+      <c r="D27">
+        <v>1</v>
+      </c>
+      <c r="F27" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A28" t="s">
+        <v>93</v>
+      </c>
+      <c r="B28" t="s">
+        <v>11</v>
+      </c>
+      <c r="C28" t="s">
+        <v>94</v>
+      </c>
+      <c r="D28">
+        <v>0</v>
+      </c>
+      <c r="F28" t="s">
+        <v>97</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="3">
     <mergeCell ref="A1:F1"/>
     <mergeCell ref="A2:F2"/>
+    <mergeCell ref="A16:F16"/>
   </mergeCells>
+  <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
Items Cart TCER added
</commit_message>
<xml_diff>
--- a/MicroService App/TCER Sheet.xlsx
+++ b/MicroService App/TCER Sheet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nagal\git\XYZRetailRepo\MicroService App\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59456DBE-CE6C-4461-A8E8-CDA1A34B432A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA0E7274-C1E4-4DD9-8348-F00DF4A6A536}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5760" yWindow="1404" windowWidth="17280" windowHeight="8880" firstSheet="1" activeTab="3" xr2:uid="{6144ADCF-C8D8-4E84-B20B-C8733E953893}"/>
+    <workbookView xWindow="5760" yWindow="1404" windowWidth="17280" windowHeight="8880" firstSheet="3" activeTab="4" xr2:uid="{6144ADCF-C8D8-4E84-B20B-C8733E953893}"/>
   </bookViews>
   <sheets>
     <sheet name="Customer Service" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="289" uniqueCount="109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="423" uniqueCount="159">
   <si>
     <t>TCER</t>
   </si>
@@ -364,6 +364,156 @@
   </si>
   <si>
     <t>if item id updated by reducing the mentioned quantity</t>
+  </si>
+  <si>
+    <t>getItemsInCart(String name)</t>
+  </si>
+  <si>
+    <t>List&lt;ItemsCart&gt;</t>
+  </si>
+  <si>
+    <t>If there is atleast one item in cart</t>
+  </si>
+  <si>
+    <t>If there is no element in the cart</t>
+  </si>
+  <si>
+    <t>deleteItemById(String customer,String itemId)</t>
+  </si>
+  <si>
+    <t>ItemsCart object</t>
+  </si>
+  <si>
+    <t>If Item exists in cart</t>
+  </si>
+  <si>
+    <t>If Item does not exists in cart</t>
+  </si>
+  <si>
+    <t>updateByItemId(String customer, String itemId, int requiredQuantity)</t>
+  </si>
+  <si>
+    <t>if item is updated succesfully</t>
+  </si>
+  <si>
+    <t>ItemCart(updated)</t>
+  </si>
+  <si>
+    <t>ItemsCart(previous)</t>
+  </si>
+  <si>
+    <t>if unable to update the item</t>
+  </si>
+  <si>
+    <t>if required quantity less than 1</t>
+  </si>
+  <si>
+    <t>T004</t>
+  </si>
+  <si>
+    <t>if item doesnot exist in cart</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> addItemtoCart(String customer, String itemId, int requiredQuantity) </t>
+  </si>
+  <si>
+    <t>ItemsCart (new object)</t>
+  </si>
+  <si>
+    <t>if item doesnot exist on cart</t>
+  </si>
+  <si>
+    <t>ItemsCart(updated item quantity and cost)</t>
+  </si>
+  <si>
+    <t>if item already exist in cart</t>
+  </si>
+  <si>
+    <t>if item unable to add to cart</t>
+  </si>
+  <si>
+    <t>deleteAllItemsInCart(String customer)</t>
+  </si>
+  <si>
+    <t>Empty ItemsCart List</t>
+  </si>
+  <si>
+    <t>If all items in cart is deleted succesfully</t>
+  </si>
+  <si>
+    <t>itemsCart List</t>
+  </si>
+  <si>
+    <t>If all items in cart is not deleted succesfully</t>
+  </si>
+  <si>
+    <t>R006</t>
+  </si>
+  <si>
+    <t>generateBill(String customer)</t>
+  </si>
+  <si>
+    <t>ItemBill object</t>
+  </si>
+  <si>
+    <t>if item is present in cart</t>
+  </si>
+  <si>
+    <t>if no items present in cart</t>
+  </si>
+  <si>
+    <t>deleteItemByItemId(@Param("id") String itemId,@Param("name") String customer)</t>
+  </si>
+  <si>
+    <t>On succesful deletion</t>
+  </si>
+  <si>
+    <t>if deletion is failed</t>
+  </si>
+  <si>
+    <t>findByItemIdAndUserName(@Param("id") String itemId,@Param("name") String userName)</t>
+  </si>
+  <si>
+    <t>Optional&lt;ItemSCart&gt;</t>
+  </si>
+  <si>
+    <t>item foiund by name</t>
+  </si>
+  <si>
+    <t>findByUserName(@Param("username") String userName)</t>
+  </si>
+  <si>
+    <t>if items exist in cart with username</t>
+  </si>
+  <si>
+    <t>if items doesnot exist in cart with username</t>
+  </si>
+  <si>
+    <t>updateByItemId(@Param("q") int requiredQuantity,@Param("cost") double totalCost,@Param("id") String itemId,@Param("name") String userName)</t>
+  </si>
+  <si>
+    <t>items cart updated succesfully</t>
+  </si>
+  <si>
+    <t>items cart not updated succesfully</t>
+  </si>
+  <si>
+    <t>addItemToCart(@Param("id") String itemId,@Param("name") String itemName,@Param("price")double unitPrice,@Param("uName")String userName,@Param("q")int requiredQuantity,@Param("tax") double salesTax,@Param("cost")double totalCost)</t>
+  </si>
+  <si>
+    <t>Item added to cart</t>
+  </si>
+  <si>
+    <t>Items unable to add</t>
+  </si>
+  <si>
+    <t>deleteAllByUserName(@Param("customer")String customer)</t>
+  </si>
+  <si>
+    <t>if all items in the cart deleted successfully</t>
+  </si>
+  <si>
+    <t>if all items in the cart not deleted successfully</t>
   </si>
 </sst>
 </file>
@@ -1649,7 +1799,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{77C7A937-846C-4C77-8D91-13859D3BE2A9}">
   <dimension ref="A1:F28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+    <sheetView topLeftCell="A7" workbookViewId="0">
       <selection activeCell="F30" sqref="F30"/>
     </sheetView>
   </sheetViews>
@@ -2018,13 +2168,20 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CADB9A91-AD13-4475-B07E-D91082D94583}">
-  <dimension ref="A1:F3"/>
+  <dimension ref="A1:F44"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:F2"/>
+    <sheetView tabSelected="1" topLeftCell="D21" workbookViewId="0">
+      <selection activeCell="F44" sqref="F44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="14.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="57.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.88671875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="28.33203125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="21" x14ac:dyDescent="0.4">
       <c r="A1" s="7" t="s">
@@ -2066,11 +2223,502 @@
         <v>14</v>
       </c>
     </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" t="s">
+        <v>109</v>
+      </c>
+      <c r="D4" t="s">
+        <v>110</v>
+      </c>
+      <c r="F4" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C5" t="s">
+        <v>109</v>
+      </c>
+      <c r="D5" t="s">
+        <v>101</v>
+      </c>
+      <c r="F5" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>13</v>
+      </c>
+      <c r="B7" t="s">
+        <v>8</v>
+      </c>
+      <c r="C7" t="s">
+        <v>113</v>
+      </c>
+      <c r="D7" t="s">
+        <v>114</v>
+      </c>
+      <c r="F7" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>13</v>
+      </c>
+      <c r="B8" t="s">
+        <v>11</v>
+      </c>
+      <c r="C8" t="s">
+        <v>113</v>
+      </c>
+      <c r="D8" t="s">
+        <v>17</v>
+      </c>
+      <c r="F8" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>22</v>
+      </c>
+      <c r="B10" t="s">
+        <v>8</v>
+      </c>
+      <c r="C10" t="s">
+        <v>117</v>
+      </c>
+      <c r="D10" t="s">
+        <v>119</v>
+      </c>
+      <c r="F10" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>22</v>
+      </c>
+      <c r="B11" t="s">
+        <v>11</v>
+      </c>
+      <c r="C11" t="s">
+        <v>117</v>
+      </c>
+      <c r="D11" t="s">
+        <v>120</v>
+      </c>
+      <c r="F11" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>22</v>
+      </c>
+      <c r="B12" t="s">
+        <v>31</v>
+      </c>
+      <c r="C12" t="s">
+        <v>117</v>
+      </c>
+      <c r="D12" t="s">
+        <v>12</v>
+      </c>
+      <c r="F12" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>22</v>
+      </c>
+      <c r="B13" t="s">
+        <v>123</v>
+      </c>
+      <c r="C13" t="s">
+        <v>117</v>
+      </c>
+      <c r="D13" t="s">
+        <v>12</v>
+      </c>
+      <c r="F13" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>27</v>
+      </c>
+      <c r="B15" t="s">
+        <v>8</v>
+      </c>
+      <c r="C15" t="s">
+        <v>125</v>
+      </c>
+      <c r="D15" t="s">
+        <v>126</v>
+      </c>
+      <c r="F15" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>27</v>
+      </c>
+      <c r="B16" t="s">
+        <v>11</v>
+      </c>
+      <c r="C16" t="s">
+        <v>125</v>
+      </c>
+      <c r="D16" t="s">
+        <v>128</v>
+      </c>
+      <c r="F16" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>27</v>
+      </c>
+      <c r="B17" t="s">
+        <v>31</v>
+      </c>
+      <c r="C17" t="s">
+        <v>125</v>
+      </c>
+      <c r="D17" t="s">
+        <v>12</v>
+      </c>
+      <c r="F17" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>27</v>
+      </c>
+      <c r="B18" t="s">
+        <v>123</v>
+      </c>
+      <c r="C18" t="s">
+        <v>125</v>
+      </c>
+      <c r="D18" t="s">
+        <v>12</v>
+      </c>
+      <c r="F18" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>59</v>
+      </c>
+      <c r="B20" t="s">
+        <v>8</v>
+      </c>
+      <c r="C20" t="s">
+        <v>131</v>
+      </c>
+      <c r="D20" t="s">
+        <v>132</v>
+      </c>
+      <c r="F20" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>59</v>
+      </c>
+      <c r="B21" t="s">
+        <v>11</v>
+      </c>
+      <c r="C21" t="s">
+        <v>131</v>
+      </c>
+      <c r="D21" t="s">
+        <v>134</v>
+      </c>
+      <c r="F21" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>136</v>
+      </c>
+      <c r="B23" t="s">
+        <v>8</v>
+      </c>
+      <c r="C23" t="s">
+        <v>137</v>
+      </c>
+      <c r="D23" t="s">
+        <v>138</v>
+      </c>
+      <c r="F23" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
+        <v>136</v>
+      </c>
+      <c r="B24" t="s">
+        <v>11</v>
+      </c>
+      <c r="C24" t="s">
+        <v>137</v>
+      </c>
+      <c r="D24" t="s">
+        <v>12</v>
+      </c>
+      <c r="F24" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" ht="18" x14ac:dyDescent="0.35">
+      <c r="A27" s="8" t="s">
+        <v>80</v>
+      </c>
+      <c r="B27" s="8"/>
+      <c r="C27" s="8"/>
+      <c r="D27" s="8"/>
+      <c r="E27" s="8"/>
+      <c r="F27" s="8"/>
+    </row>
+    <row r="28" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A28" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D28" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E28" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F28" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A29" t="s">
+        <v>7</v>
+      </c>
+      <c r="B29" t="s">
+        <v>8</v>
+      </c>
+      <c r="C29" t="s">
+        <v>141</v>
+      </c>
+      <c r="D29">
+        <v>1</v>
+      </c>
+      <c r="F29" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A30" t="s">
+        <v>7</v>
+      </c>
+      <c r="B30" t="s">
+        <v>11</v>
+      </c>
+      <c r="C30" t="s">
+        <v>141</v>
+      </c>
+      <c r="D30">
+        <v>0</v>
+      </c>
+      <c r="F30" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A32" t="s">
+        <v>13</v>
+      </c>
+      <c r="B32" t="s">
+        <v>8</v>
+      </c>
+      <c r="C32" t="s">
+        <v>144</v>
+      </c>
+      <c r="D32" t="s">
+        <v>145</v>
+      </c>
+      <c r="F32" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A34" t="s">
+        <v>22</v>
+      </c>
+      <c r="B34" t="s">
+        <v>8</v>
+      </c>
+      <c r="C34" t="s">
+        <v>147</v>
+      </c>
+      <c r="D34" t="s">
+        <v>110</v>
+      </c>
+      <c r="F34" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A35" t="s">
+        <v>22</v>
+      </c>
+      <c r="B35" t="s">
+        <v>11</v>
+      </c>
+      <c r="C35" t="s">
+        <v>147</v>
+      </c>
+      <c r="D35" t="s">
+        <v>101</v>
+      </c>
+      <c r="F35" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A37" t="s">
+        <v>27</v>
+      </c>
+      <c r="B37" t="s">
+        <v>8</v>
+      </c>
+      <c r="C37" t="s">
+        <v>150</v>
+      </c>
+      <c r="D37">
+        <v>1</v>
+      </c>
+      <c r="F37" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A38" t="s">
+        <v>27</v>
+      </c>
+      <c r="B38" t="s">
+        <v>11</v>
+      </c>
+      <c r="C38" t="s">
+        <v>150</v>
+      </c>
+      <c r="D38">
+        <v>0</v>
+      </c>
+      <c r="F38" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A40" t="s">
+        <v>59</v>
+      </c>
+      <c r="B40" t="s">
+        <v>8</v>
+      </c>
+      <c r="C40" t="s">
+        <v>153</v>
+      </c>
+      <c r="D40">
+        <v>1</v>
+      </c>
+      <c r="F40" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A41" t="s">
+        <v>59</v>
+      </c>
+      <c r="B41" t="s">
+        <v>11</v>
+      </c>
+      <c r="C41" t="s">
+        <v>153</v>
+      </c>
+      <c r="D41">
+        <v>0</v>
+      </c>
+      <c r="F41" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A43" t="s">
+        <v>136</v>
+      </c>
+      <c r="B43" t="s">
+        <v>8</v>
+      </c>
+      <c r="C43" t="s">
+        <v>156</v>
+      </c>
+      <c r="D43">
+        <v>1</v>
+      </c>
+      <c r="F43" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A44" t="s">
+        <v>136</v>
+      </c>
+      <c r="B44" t="s">
+        <v>11</v>
+      </c>
+      <c r="C44" t="s">
+        <v>156</v>
+      </c>
+      <c r="D44">
+        <v>0</v>
+      </c>
+      <c r="F44" t="s">
+        <v>158</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="3">
     <mergeCell ref="A1:F1"/>
     <mergeCell ref="A2:F2"/>
+    <mergeCell ref="A27:F27"/>
   </mergeCells>
+  <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>